<commit_message>
updating examples output files following aneuploidy event size fix
</commit_message>
<xml_diff>
--- a/examples/Sample8_vs_HG002/Sample8_vs_HG002.xlsx
+++ b/examples/Sample8_vs_HG002/Sample8_vs_HG002.xlsx
@@ -2400,8 +2400,10 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>180507680</v>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="J2" s="2" t="n">
         <v>2.695</v>
@@ -2458,8 +2460,10 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="I3" s="2" t="n">
-        <v>128439889</v>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="J3" s="2" t="n">
         <v>2.376</v>
@@ -2516,8 +2520,10 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="I4" s="2" t="n">
-        <v>37520123</v>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="J4" s="2" t="n">
         <v>2.347</v>

</xml_diff>

<commit_message>
updating examples output files
</commit_message>
<xml_diff>
--- a/examples/Sample8_vs_HG002/Sample8_vs_HG002.xlsx
+++ b/examples/Sample8_vs_HG002/Sample8_vs_HG002.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,37 +1766,37 @@
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>duplication_split</t>
+          <t>insertion</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>72436529</v>
+        <v>93690639</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>72668687</v>
+        <v>93707149</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>232158</v>
+        <v>5722</v>
       </c>
       <c r="J26" s="2" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L26" s="2" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1823,28 +1823,28 @@
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F27" s="2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="G27" s="2" t="n">
-        <v>93690639</v>
+        <v>54210155</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>93707149</v>
+        <v>54219148</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>5722</v>
+        <v>6089</v>
       </c>
       <c r="J27" s="2" t="n">
-        <v>19</v>
+        <v>93</v>
       </c>
       <c r="K27" s="2" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L27" s="2" t="inlineStr">
         <is>
@@ -1875,28 +1875,28 @@
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>54210155</v>
+        <v>148336764</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>54219148</v>
+        <v>148348351</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>6089</v>
+        <v>23955</v>
       </c>
       <c r="J28" s="2" t="n">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="L28" s="2" t="inlineStr">
         <is>
@@ -1927,32 +1927,32 @@
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G29" s="2" t="n">
-        <v>148336764</v>
+        <v>76832500</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>148348351</v>
+        <v>76851752</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>23955</v>
+        <v>12613</v>
       </c>
       <c r="J29" s="2" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L29" s="2" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1974,30 +1974,32 @@
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>insertion</t>
+          <t>translocation_interchr</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>19</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>76832500</v>
+        <v>118493942</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>76851752</v>
-      </c>
-      <c r="I30" s="2" t="n">
-        <v>12613</v>
+        <v>6276713</v>
+      </c>
+      <c r="I30" s="2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="J30" s="2" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K30" s="2" t="n">
         <v>0</v>
@@ -2031,19 +2033,19 @@
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>20</t>
         </is>
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>21</t>
         </is>
       </c>
       <c r="G31" s="2" t="n">
-        <v>118493942</v>
+        <v>32720656</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>6276713</v>
+        <v>43652112</v>
       </c>
       <c r="I31" s="2" t="inlineStr">
         <is>
@@ -2051,7 +2053,7 @@
         </is>
       </c>
       <c r="J31" s="2" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K31" s="2" t="n">
         <v>0</v>
@@ -2085,7 +2087,7 @@
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F32" s="2" t="inlineStr">
@@ -2094,10 +2096,10 @@
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>32720656</v>
+        <v>101137685</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>43652112</v>
+        <v>33583687</v>
       </c>
       <c r="I32" s="2" t="inlineStr">
         <is>
@@ -2105,7 +2107,7 @@
         </is>
       </c>
       <c r="J32" s="2" t="n">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="K32" s="2" t="n">
         <v>0</v>
@@ -2139,19 +2141,19 @@
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="G33" s="2" t="n">
-        <v>101137685</v>
+        <v>130764655</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>33583687</v>
+        <v>23236212</v>
       </c>
       <c r="I33" s="2" t="inlineStr">
         <is>
@@ -2159,10 +2161,10 @@
         </is>
       </c>
       <c r="J33" s="2" t="n">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="K33" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" s="2" t="inlineStr">
         <is>
@@ -2188,24 +2190,24 @@
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>translocation_interchr</t>
+          <t>translocation_intrachr</t>
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>130764655</v>
+        <v>74489342</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>23236212</v>
+        <v>126887290</v>
       </c>
       <c r="I34" s="2" t="inlineStr">
         <is>
@@ -2213,66 +2215,12 @@
         </is>
       </c>
       <c r="J34" s="2" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="K34" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L34" s="2" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>HCM</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>Sample8</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="inlineStr">
-        <is>
-          <t>HG002</t>
-        </is>
-      </c>
-      <c r="D35" s="2" t="inlineStr">
-        <is>
-          <t>translocation_intrachr</t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="F35" s="2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="G35" s="2" t="n">
-        <v>74489342</v>
-      </c>
-      <c r="H35" s="2" t="n">
-        <v>126887290</v>
-      </c>
-      <c r="I35" s="2" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="J35" s="2" t="n">
-        <v>49</v>
-      </c>
-      <c r="K35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" s="2" t="inlineStr">
         <is>
           <t>no</t>
         </is>

</xml_diff>